<commit_message>
atualização da tabela de riscos
</commit_message>
<xml_diff>
--- a/sprint_grupo7/PI/Tabela de riscos.xlsx
+++ b/sprint_grupo7/PI/Tabela de riscos.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E9A2FE4-0A20-4236-8CC5-8995377CF637}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiag\OneDrive\Documentos\Pesquisa e inovação\sprint_01\sprint_grupo7\PI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008532C1-F654-49B1-8429-29475129FC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,18 +44,9 @@
     <t>Descrição do risco</t>
   </si>
   <si>
-    <t>Probabilidade (P)    1 - Baixa                       2 - Média              3 - Alta</t>
-  </si>
-  <si>
-    <t>Impacto (i)   1 - Baixa        2 - Média       3 - Alta</t>
-  </si>
-  <si>
     <t>Fator de Risco              (P) x (I)</t>
   </si>
   <si>
-    <t>Ação            -Evitar          -Mitigar</t>
-  </si>
-  <si>
     <t>Como?</t>
   </si>
   <si>
@@ -103,13 +99,22 @@
   </si>
   <si>
     <t>Buscar outros meios de poder seguir com o projeto por outros meios.</t>
+  </si>
+  <si>
+    <t>Probabilidade (P)    1 - Baixa                       2 - Média                        3 - Alta</t>
+  </si>
+  <si>
+    <t>Impacto (i)         1 - Baixa               2 - Média              3 - Alta</t>
+  </si>
+  <si>
+    <t>Ação                 -Evitar             -Mitigar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +126,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -170,37 +183,6 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -209,90 +191,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -310,11 +210,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -322,140 +272,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -475,35 +342,117 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color rgb="FF000000"/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -517,7 +466,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -540,6 +489,28 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -554,23 +525,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D2890073-F056-483B-B8AD-52175A92E886}" name="Tabela1" displayName="Tabela1" ref="B1:H9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="B1:H9" xr:uid="{D2890073-F056-483B-B8AD-52175A92E886}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D2890073-F056-483B-B8AD-52175A92E886}" name="Tabela1" displayName="Tabela1" ref="B1:H16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="B1:H16" xr:uid="{D2890073-F056-483B-B8AD-52175A92E886}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2DC47522-C6B2-4CB4-AF9F-16DF27B4872D}" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{5D9E9B77-9A5D-4D05-8A51-AEBCA09DE655}" name="Descrição do risco" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{88239A24-23A2-4B1D-8127-7A14167D3010}" name="Probabilidade (P)    1 - Baixa                       2 - Média              3 - Alta" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{F8C5182D-97F6-468D-937A-5037A9BF46E2}" name="Impacto (i)   1 - Baixa        2 - Média       3 - Alta" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{0BBAB1E8-B6D4-47EE-B2E3-05B26004DC93}" name="Fator de Risco              (P) x (I)" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{B926D3C6-3BBB-4F2C-AA27-4A0172ABA5C3}" name="Ação            -Evitar          -Mitigar" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{4896C8CE-9E0B-4DFB-A2A4-1D27090336FB}" name="Como?" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2DC47522-C6B2-4CB4-AF9F-16DF27B4872D}" name="ID" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{5D9E9B77-9A5D-4D05-8A51-AEBCA09DE655}" name="Descrição do risco" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{88239A24-23A2-4B1D-8127-7A14167D3010}" name="Probabilidade (P)    1 - Baixa                       2 - Média                        3 - Alta" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{F8C5182D-97F6-468D-937A-5037A9BF46E2}" name="Impacto (i)         1 - Baixa               2 - Média              3 - Alta" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{0BBAB1E8-B6D4-47EE-B2E3-05B26004DC93}" name="Fator de Risco              (P) x (I)" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{B926D3C6-3BBB-4F2C-AA27-4A0172ABA5C3}" name="Ação                 -Evitar             -Mitigar" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{4896C8CE-9E0B-4DFB-A2A4-1D27090336FB}" name="Como?" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -866,273 +837,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J12"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.33203125" customWidth="1"/>
+    <col min="9" max="9" width="47.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="60.75">
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="G1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>6</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B2" s="12">
+    <row r="2" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="14">
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13">
         <v>2</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>2</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <v>4</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B3" s="6">
+    <row r="3" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="17">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="13">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="13">
         <v>3</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="13">
         <v>3</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>10</v>
+      <c r="G3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B4" s="6">
+    <row r="4" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="14">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="13">
         <v>3</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="13">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
+      <c r="G4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="2:10" ht="30" customHeight="1">
-      <c r="B5" s="6">
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="13">
+        <v>2</v>
+      </c>
+      <c r="E5" s="13">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13">
+        <v>6</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="14">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3">
-        <v>2</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="2:10" ht="45.75">
-      <c r="B6" s="6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3">
-        <v>4</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:10" ht="60.75">
-      <c r="B7" s="6">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="14">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="13">
         <v>3</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="13">
         <v>3</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>19</v>
+      <c r="G7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B8" s="6">
+    <row r="8" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="13">
         <v>1</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="13">
         <v>2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="13">
         <v>1</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>21</v>
+      <c r="G8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1">
-      <c r="B9" s="17">
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14">
         <v>8</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="19">
+      <c r="C9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="13">
         <v>2</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="13">
         <v>3</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="13">
         <v>6</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>23</v>
+      <c r="G9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B10" s="8"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+    <row r="10" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="14">
+        <v>10</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="14">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="14">
+        <v>12</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="15">
+        <v>15</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" ht="57.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>